<commit_message>
New .md files to keep track of things, restructuring
</commit_message>
<xml_diff>
--- a/nanDECK/Cards/Minister of Commerce/Minister of Commerce.xlsx
+++ b/nanDECK/Cards/Minister of Commerce/Minister of Commerce.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4877ff4c3120fcf5/board game design/Space Roles Game/nanDECK/Cards/Minister of Commerce/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\keremataman\GitHub\kardashev-scale\nanDECK\Cards\Minister of Commerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="11_F25DC773A252ABDACC1048E5A95D6B645ADE58EF" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0EFA3818-D08A-46A6-BD84-754C18AAB5DD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8377C8-BDC5-4B57-B5E3-5AB5D586AC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8190" yWindow="1410" windowWidth="20610" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -39,30 +39,15 @@
     <t>Text</t>
   </si>
   <si>
-    <t>Shill</t>
-  </si>
-  <si>
     <t>Basic Action</t>
   </si>
   <si>
-    <t>Gain twice as much money from your reserve workers at the end of your turn</t>
-  </si>
-  <si>
-    <t>Recruit</t>
-  </si>
-  <si>
-    <t>Add 1 unit from the worker reserve to your worker pool</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
     <t>Financial Restructuring</t>
   </si>
   <si>
-    <t>You may move X gold from one player to another, where X is the number of workers you committed to this action</t>
-  </si>
-  <si>
     <t>Marilyn Campaign</t>
   </si>
   <si>
@@ -78,82 +63,77 @@
     <t>Predicting the Market</t>
   </si>
   <si>
-    <t>X is the number of players
+    <t>Adonis Campaign</t>
+  </si>
+  <si>
+    <t>Eve Campaign</t>
+  </si>
+  <si>
+    <t>Rex Campaign</t>
+  </si>
+  <si>
+    <t>Launch Campaign</t>
+  </si>
+  <si>
+    <t>Campaign</t>
+  </si>
+  <si>
+    <t>Balancing the Books</t>
+  </si>
+  <si>
+    <t>Creative Accounting</t>
+  </si>
+  <si>
+    <t>BG Image</t>
+  </si>
+  <si>
+    <t>Minister of Commerce.jpg</t>
+  </si>
+  <si>
+    <t>You may move any amount of Gold between Players</t>
+  </si>
+  <si>
+    <t>When you play this card, place 6 Gold on it. This card stays on the field until there is no more Gold on it
+At the start of your turn, take 2 Gold from this card. If there is no Gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
+  </si>
+  <si>
+    <t>When you play this card, place 8 Gold on it. This card stays on the field until there is no more Gold on it
+At the start of your turn, take 2 Gold from this card. If there is no Gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
+  </si>
+  <si>
+    <t>When you place this card, place X tradable goods on it. This card stays on the field until there is no more tradable goods on it
+At the start of your turn, remove 1 tradable good from this card and gain 3 Gold. If there are no tradable goods remaining on this card, shuffle it back into MoC's deck</t>
+  </si>
+  <si>
+    <t>When you play this card, place 12 Gold on it. This card stays on the field until there is no more Gold on it
+At the start of your turn, take 3 Gold from this card. If there is no Gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
+  </si>
+  <si>
+    <t>When you play this card, place 16 Gold on it. This card stays on the field until there is no more Gold on it
+At the start of your turn, take 2 Gold from this card. If there is no Gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
+  </si>
+  <si>
+    <t>Until your next turn, Players may spend Tradable Goods instead of Money</t>
+  </si>
+  <si>
+    <t>When you play this card, choose a Player other than yourself, then place X Gold on this card
+Guess whether the dice roll of the Player will be successful or not in their next turn. If you are correct, gain 2X Gold. If your prediction is incorrect or if the Player does not roll a dice, lose the Gold spent on this dice.
+Once the selected Player completes their turn, shuffle this card back into the MoC's deck</t>
+  </si>
+  <si>
+    <t>X is the number of Players
 When you play this card, shuffle it into the event deck
-When this card is drawn from the event deck, each player doubles their money. Then, shuffle this card into minister of commerce's deck</t>
-  </si>
-  <si>
-    <t>Adonis Campaign</t>
-  </si>
-  <si>
-    <t>Eve Campaign</t>
-  </si>
-  <si>
-    <t>Rex Campaign</t>
-  </si>
-  <si>
-    <t>Launch Campaign</t>
-  </si>
-  <si>
-    <t>Campaign</t>
-  </si>
-  <si>
-    <t>Balancing the Books</t>
-  </si>
-  <si>
-    <t>When you play this card, choose a player other than yourself, then place X gold on this card
-Guess whether the dice roll of the player will be successful or not in their next turn. If you are correct, gain 2X gold. If your prediction is incorrect or if the player does not roll a dice, lose the gold spent on this dice.
-Once the selected player completes their turn, shuffle this card back into the MoC's deck</t>
-  </si>
-  <si>
-    <t>When you play this card, choose a player other than yourself, then place X gold on this card
-Guess the name of the card the player will play in their next turn. If you guess correctly, gain 2X gold, otherwise, lose all the gold you placed on this card
-Once the selected player completes their turn, shuffle this card back into the MoC's deck</t>
-  </si>
-  <si>
-    <t>When you play this card, choose a player other than yourself, then place X gold on this card
-In their next turn, if the player spends or gains X gold from the beginning of their turn until the end of their turn, receive 2X gold.
-Once the selected player completes their turn, shuffle this card back into the MoC's deck</t>
-  </si>
-  <si>
-    <t>When you play this card, choose a player other than yourself, then place X gold on this card
-If the selected player has X uncommited workers at the end of their next turn, receive 2X gold.
-Once the selected player completes their turn, shuffle this card back into the MoC's deck</t>
-  </si>
-  <si>
-    <t>Allocating Workforce</t>
-  </si>
-  <si>
-    <t>Until your next turn, players may spend tradable goods instead of money</t>
-  </si>
-  <si>
-    <t>Creative Accounting</t>
-  </si>
-  <si>
-    <t>When you play this card, place 6 gold on it. This card stays on the field until there is no more gold on it
-At the start of your turn, take 2 gold from this card. If there is no gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
-  </si>
-  <si>
-    <t>When you play this card, place 8 gold on it. This card stays on the field until there is no more gold on it
-At the start of your turn, take 2 gold from this card. If there is no gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
-  </si>
-  <si>
-    <t>When you place this card, place X tradable goods on it. This card stays on the field until there is no more tradable goods on it
-At the start of your turn, remove 1 tradable good from this card and gain 3 gold. If there are no tradable goods remaining on this card, shuffle it back into MoC's deck</t>
-  </si>
-  <si>
-    <t>When you play this card, place 12 gold on it. This card stays on the field until there is no more gold on it
-At the start of your turn, take 3 gold from this card. If there is no gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
-  </si>
-  <si>
-    <t>When you play this card, place 16 gold on it. This card stays on the field until there is no more gold on it
-At the start of your turn, take 2 gold from this card. If there is no gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
-  </si>
-  <si>
-    <t>BG Image</t>
-  </si>
-  <si>
-    <t>Minister of Commerce.jpg</t>
+When this card is drawn from the event deck, each Player doubles their money. Then, shuffle this card into MoC's deck</t>
+  </si>
+  <si>
+    <t>When you play this card, choose a Player other than yourself, then place X Gold on this card
+Guess the name of a card the Player will play in their next turn. If you guess correctly, gain 2X Gold, otherwise, lose all the Gold you placed on this card
+Once the selected Player completes their turn, shuffle this card back into the MoC's deck</t>
+  </si>
+  <si>
+    <t>When you play this card, choose a Player other than yourself, then place X Gold on this card
+In their next turn, if the Player spends or gains X Gold at some point in their next turn, receive 2X Gold, otherwise, lose all the Gold you placed on this card
+Once the selected Player completes their turn, shuffle this card back into the MoC's deck</t>
   </si>
 </sst>
 </file>
@@ -169,12 +149,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -189,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -198,6 +184,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -480,17 +473,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="147.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="100.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -498,7 +491,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -512,87 +505,87 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -600,166 +593,115 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>